<commit_message>
Added entries on CSV file
Added entries on CSV file
</commit_message>
<xml_diff>
--- a/positions.VioletSorrengail.xlsx
+++ b/positions.VioletSorrengail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/582a54d420dfddd6/Documents/paf-14-cv-lab-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{30980217-07DF-42AC-B0A3-02567049D4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18683D4B-6694-4A15-8F7A-62B8729FFF50}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{30980217-07DF-42AC-B0A3-02567049D4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBC50AE8-664A-4724-8604-841C8D25CEB0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B551C5A-2A69-4361-A361-8428615F7493}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="positions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">positions!$A$4:$J$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">positions!$A$5:$J$14</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
   <si>
     <t>section</t>
   </si>
@@ -67,9 +67,6 @@
     <t>data_science_writings</t>
   </si>
   <si>
-    <t>Contracted article.</t>
-  </si>
-  <si>
     <t>about_me_press</t>
   </si>
   <si>
@@ -143,6 +140,48 @@
   </si>
   <si>
     <t>First person excerpts of dealing with Tairn and Andarna provided by Violet</t>
+  </si>
+  <si>
+    <t>How to cope with having your once deceased brother be not deceased</t>
+  </si>
+  <si>
+    <t>First person excepts of Violet finiding out that her brother who was once though dead is actually alive and part of the rebellion you were once taught to hate and fight against</t>
+  </si>
+  <si>
+    <t>First rider to be chosen by two dragons</t>
+  </si>
+  <si>
+    <t>Story of how Violet was chosen by Tairn and Andarna, both incredibly rare dragons, not to mention Tairn's pairing with Sgaeyl</t>
+  </si>
+  <si>
+    <t>Being Xaden Riorson's Partner: Blessing or a Cruse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What it is like being Xaden Riorson's partner as well as sharing mated dragons. Advise for future riders and who *not* to chose </t>
+  </si>
+  <si>
+    <t>Vlog written after Xaden's post orders</t>
+  </si>
+  <si>
+    <t>Restricted files</t>
+  </si>
+  <si>
+    <t>Voted Second Squads Most Improved Cadet</t>
+  </si>
+  <si>
+    <t>Position given as recipient was expected to fail during the first challenge and instead, became the most powerful dragon rider</t>
+  </si>
+  <si>
+    <t>Sorrengail Family Tree</t>
+  </si>
+  <si>
+    <t>Addendum provided by scribes: Family tree was ripped out in 2017 after Violet and Mira's treason to Navarre</t>
+  </si>
+  <si>
+    <t>Certificate For Being the Most Hated Second Year Rider</t>
+  </si>
+  <si>
+    <t>Awarded for being the most hated rider, including mulyiple attempts on her life by other unbonded riders/cadets</t>
   </si>
 </sst>
 </file>
@@ -684,6 +723,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1003,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55333E2C-D43B-4655-99E5-5C4A93A5AF8E}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,13 +1104,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
       </c>
       <c r="F2">
         <v>2015</v>
@@ -1076,7 +1119,7 @@
         <v>2020</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -1093,45 +1136,42 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
       <c r="F3">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="G3">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
       <c r="F4">
         <v>2011</v>
@@ -1140,7 +1180,7 @@
         <v>2015</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -1151,19 +1191,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
       </c>
       <c r="F5">
         <v>2011</v>
@@ -1172,7 +1212,7 @@
         <v>2015</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -1183,31 +1223,31 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>2011</v>
       </c>
       <c r="G6">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
@@ -1215,31 +1255,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>2011</v>
       </c>
       <c r="G7">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
@@ -1247,31 +1287,31 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8">
+        <v>2014</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
         <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
@@ -1279,38 +1319,230 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>2015</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>2014</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>2017</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>2016</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>2015</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>2016</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9">
-        <v>2016</v>
-      </c>
-      <c r="G9">
-        <v>2016</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>2017</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J9" xr:uid="{55333E2C-D43B-4655-99E5-5C4A93A5AF8E}"/>
+  <autoFilter ref="A5:J14" xr:uid="{55333E2C-D43B-4655-99E5-5C4A93A5AF8E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>